<commit_message>
Latest City Pal Application
</commit_message>
<xml_diff>
--- a/Client Requirements.xlsx
+++ b/Client Requirements.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacob/Documents/Uni/2017/Sem 2/IFB299/Assessment 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/William/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8120" yWindow="0" windowWidth="13760" windowHeight="20920" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,14 +27,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
   <si>
     <t>Features</t>
   </si>
   <si>
-    <t>Y or N</t>
-  </si>
-  <si>
     <t>Geo location</t>
   </si>
   <si>
@@ -59,9 +56,6 @@
     <t>Customised GUI to user</t>
   </si>
   <si>
-    <t>j.stgermain@qut.edu.au</t>
-  </si>
-  <si>
     <t>User related to</t>
   </si>
   <si>
@@ -71,6 +65,9 @@
     <t>City info</t>
   </si>
   <si>
+    <t>Ability to view other use info types</t>
+  </si>
+  <si>
     <t>Simplified user acc creation</t>
   </si>
   <si>
@@ -95,9 +92,6 @@
     <t>Emergency services</t>
   </si>
   <si>
-    <t>Better user exp</t>
-  </si>
-  <si>
     <t xml:space="preserve">Help build community </t>
   </si>
   <si>
@@ -153,24 +147,12 @@
   </si>
   <si>
     <t>Admin</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Ability to view other user info types</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -217,16 +199,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -505,18 +483,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="95" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.33203125" customWidth="1"/>
     <col min="2" max="2" width="33.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="3"/>
-    <col min="4" max="4" width="17.1640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -525,293 +503,227 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>11</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>40</v>
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>40</v>
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>40</v>
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>41</v>
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>40</v>
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>40</v>
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>40</v>
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>40</v>
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>40</v>
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>40</v>
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>40</v>
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>40</v>
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>40</v>
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>40</v>
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>17</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F36" s="4"/>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A23" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>